<commit_message>
manual paper annotation results
</commit_message>
<xml_diff>
--- a/paper-annotation/2._annotations_pilot_jg.xlsx
+++ b/paper-annotation/2._annotations_pilot_jg.xlsx
@@ -832,7 +832,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1641,7 +1641,7 @@
         <v>42</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32">

</xml_diff>